<commit_message>
Updated requirements - added check for dpf app
</commit_message>
<xml_diff>
--- a/Smash - requriements.xlsx
+++ b/Smash - requriements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viaucdk-my.sharepoint.com/personal/331187_viauc_dk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viaucdk-my.sharepoint.com/personal/331187_viauc_dk/Documents/smashpadelcenter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{90E71A6A-37F0-490D-81B6-DAD5700871B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F4D472-B608-4B6A-9F6A-17D2994EC1E8}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{90E71A6A-37F0-490D-81B6-DAD5700871B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79DD9248-1EA8-4992-B27F-E39BBBFD44E1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{AA181706-D876-4FBC-946A-80ADC87F6784}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Requirements</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>DPF - System (Web app) - Authentication Keycloak</t>
+  </si>
+  <si>
+    <t>DPF - Registrering ved ankomst</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF6292A-80B6-488A-B92F-FF973FA2B9E2}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:O22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,7 +543,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -551,6 +554,9 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -560,9 +566,6 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -573,7 +576,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -584,6 +587,9 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -602,9 +608,6 @@
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -615,7 +618,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -626,6 +629,9 @@
       <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -653,9 +659,6 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -666,7 +669,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -678,7 +681,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -690,7 +693,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -702,7 +705,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -714,7 +717,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -726,7 +729,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -738,7 +741,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -750,7 +753,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -762,53 +765,65 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I1:O22"/>
+    <mergeCell ref="I1:O23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>